<commit_message>
KAHI Session 2 Update
</commit_message>
<xml_diff>
--- a/data/KAHI_class_self_1.xlsx
+++ b/data/KAHI_class_self_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/KAHI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/KAHI/participant_1_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46B24611-AEC6-DB49-84D4-0247EB3C1662}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C379822-94B3-904B-A47A-F7A1AB65D424}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39500" yWindow="9160" windowWidth="26040" windowHeight="13800" xr2:uid="{BCB8E06C-46BF-A54F-84A7-1F15C3694C88}"/>
+    <workbookView xWindow="39420" yWindow="8540" windowWidth="26040" windowHeight="13800" xr2:uid="{BCB8E06C-46BF-A54F-84A7-1F15C3694C88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Question</t>
   </si>
@@ -87,13 +87,22 @@
   </si>
   <si>
     <t>Easily bothered by lights/screens or noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A little worse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somewhat worse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A lot worse </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -441,10 +450,10 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
@@ -452,7 +461,7 @@
     <col min="4" max="4" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,74 +475,116 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>